<commit_message>
ekspor + input data user done
</commit_message>
<xml_diff>
--- a/public/assets/import_format.xlsx
+++ b/public/assets/import_format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ekoperasi\public\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gawean\LAB\ekoperasi\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CE1261-A5D6-4E10-8FF0-3CE1E3776608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C37F3C-FDBA-43D1-9AFA-F7BDDEDC77B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{BAA6FBA3-7918-484E-A823-DFD1AE569BC1}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{BAA6FBA3-7918-484E-A823-DFD1AE569BC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -66,6 +58,15 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>saldo pokok</t>
+  </si>
+  <si>
+    <t>saldo wajib</t>
+  </si>
+  <si>
+    <t>saldo manasuka</t>
   </si>
 </sst>
 </file>
@@ -438,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0CCBEF-79F3-408A-A4B2-00322AE58C15}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K11"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +457,7 @@
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,68 +491,77 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
       <c r="F2" s="3"/>
       <c r="J2" s="4"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="F3" s="3"/>
       <c r="J3" s="4"/>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="F4" s="3"/>
       <c r="J4" s="4"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="F5" s="3"/>
       <c r="J5" s="4"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="F6" s="3"/>
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="F7" s="3"/>
       <c r="J7" s="4"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="F8" s="3"/>
       <c r="J8" s="4"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="F9" s="3"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="F10" s="3"/>
       <c r="J10" s="4"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="F11" s="3"/>
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
     </row>
   </sheetData>

</xml_diff>